<commit_message>
Post adding of adjustments functionality
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,22 +488,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>61</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>67</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>accounts_receivable</t>
+          <t>ar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -525,22 +525,392 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>112</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>125</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>140</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Current Assets</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>current_assets_subtotal</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>186</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Property, Plant &amp; Equipment</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ppe</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>331</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Assets</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>total_assets</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>482</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>517</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>554</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Accounts Payable</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Long-Term Debt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>debt</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Liabilities</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>total_liabilities</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Common Stock</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>common_stock</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>retained_earnings</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1,035</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2,180</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3,527</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>5,114</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>7,039</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Equity</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>total_equity</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1,135</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2,280</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3,627</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>5,214</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>7,139</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Liabilities &amp; Equity</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>total_liabs_equity</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1,365</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2,510</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3,867</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>5,464</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>7,399</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor financial statement model: update forecast method terminology, enhance configuration validation, and streamline imports. Remove deprecated modules and improve documentation clarity. Ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
@@ -816,27 +816,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,035</t>
+          <t>1,055</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2,180</t>
+          <t>2,200</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3,527</t>
+          <t>3,553</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5,114</t>
+          <t>5,154</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7,039</t>
+          <t>7,064</t>
         </is>
       </c>
     </row>
@@ -853,27 +853,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,135</t>
+          <t>1,155</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,280</t>
+          <t>2,300</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3,627</t>
+          <t>3,653</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5,214</t>
+          <t>5,254</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7,139</t>
+          <t>7,164</t>
         </is>
       </c>
     </row>
@@ -890,27 +890,27 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1,365</t>
+          <t>1,385</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2,510</t>
+          <t>2,530</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3,867</t>
+          <t>3,892</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5,464</t>
+          <t>5,503</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7,399</t>
+          <t>7,424</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor concatenate_script and update examples: improve code formatting, enhance documentation, and ensure consistent use of logging. Remove deprecated demo scripts and streamline configuration handling across examples. Ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>2026</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -506,6 +511,7 @@
           <t>67</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -543,6 +549,7 @@
           <t>140</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -580,6 +587,7 @@
           <t>207</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -617,6 +625,7 @@
           <t>347</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -654,6 +663,7 @@
           <t>554</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -691,6 +701,7 @@
           <t>101</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -728,6 +739,7 @@
           <t>159</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -765,6 +777,7 @@
           <t>260</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -802,6 +815,7 @@
           <t>100</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -816,29 +830,30 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,055</t>
+          <t>1,305</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2,200</t>
+          <t>2,500</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3,553</t>
+          <t>3,894</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5,154</t>
+          <t>5,552</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7,064</t>
-        </is>
-      </c>
+          <t>7,517</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -853,29 +868,30 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,155</t>
+          <t>1,405</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,300</t>
+          <t>2,600</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3,653</t>
+          <t>3,994</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5,254</t>
+          <t>5,652</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7,164</t>
-        </is>
-      </c>
+          <t>7,617</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -890,29 +906,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1,385</t>
+          <t>1,635</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2,530</t>
+          <t>2,830</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3,892</t>
+          <t>4,233</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5,503</t>
+          <t>5,901</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7,424</t>
-        </is>
-      </c>
+          <t>7,877</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update financial statements and enhance configuration handling: Adjust financial statement values for accuracy, improve error handling in the transformation process, and streamline import statements across modules. Ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,11 +469,6 @@
           <t>2026</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>units</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -511,7 +506,6 @@
           <t>67</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -549,7 +543,6 @@
           <t>140</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -587,7 +580,6 @@
           <t>207</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -625,7 +617,6 @@
           <t>347</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -663,7 +654,6 @@
           <t>554</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -701,7 +691,6 @@
           <t>101</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -739,7 +728,6 @@
           <t>159</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -777,7 +765,6 @@
           <t>260</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -815,7 +802,6 @@
           <t>100</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -840,20 +826,19 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3,894</t>
+          <t>3,912</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5,552</t>
+          <t>5,558</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7,517</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
+          <t>7,543</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -878,20 +863,19 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3,994</t>
+          <t>4,012</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5,652</t>
+          <t>5,658</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7,617</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
+          <t>7,643</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -916,20 +900,19 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4,233</t>
+          <t>4,251</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5,901</t>
+          <t>5,908</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7,877</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
+          <t>7,903</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor income statement generation and configuration handling: remove YAML configuration files in favor of code-based statement structure, enhance logging for statement generation, and ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/balance_sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,111 +806,148 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Retained Earnings</t>
+          <t xml:space="preserve">  Net Income</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>retained_earnings</t>
+          <t>net_income</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,305</t>
+          <t>1,525</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2,500</t>
+          <t>1,850</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3,912</t>
+          <t>2,116</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5,558</t>
+          <t>2,429</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7,543</t>
+          <t>2,799</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Equity</t>
+          <t xml:space="preserve">  Retained Earnings</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>total_equity</t>
+          <t>retained_earnings</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,405</t>
+          <t>1,635</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,600</t>
+          <t>2,905</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4,012</t>
+          <t>4,316</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5,658</t>
+          <t>5,984</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7,643</t>
+          <t>7,982</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t xml:space="preserve">  Total Equity</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>total_equity</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1,735</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3,005</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4,416</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>6,084</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>8,082</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t xml:space="preserve">  Total Liabilities &amp; Equity</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>total_liabs_equity</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1,635</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2,830</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>4,251</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>5,908</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>7,903</t>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1,965</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3,235</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>4,656</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>6,333</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8,342</t>
         </is>
       </c>
     </row>

</xml_diff>